<commit_message>
Update user ID in dashboard to reflect new contact number and modify expenses spreadsheet
</commit_message>
<xml_diff>
--- a/data/expenses/+94760937443_expenses.xlsx
+++ b/data/expenses/+94760937443_expenses.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>millennium</t>
+  </si>
+  <si>
+    <t>Shopping at</t>
+  </si>
+  <si>
+    <t>kzon</t>
   </si>
 </sst>
 </file>
@@ -417,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="15" customWidth="1"/>
@@ -453,6 +459,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>350</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Add Google Sheets integration component and update dependencies for Google Cloud and APIs
</commit_message>
<xml_diff>
--- a/data/expenses/+94760937443_expenses.xlsx
+++ b/data/expenses/+94760937443_expenses.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>kzon</t>
+  </si>
+  <si>
+    <t>2025-03-25</t>
   </si>
 </sst>
 </file>
@@ -423,7 +426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="15" customWidth="1"/>
@@ -473,6 +476,48 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>350</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>350</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>350</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>